<commit_message>
bug in generating futures.
</commit_message>
<xml_diff>
--- a/files/emergency_domain/jan_2011_calls.xlsx
+++ b/files/emergency_domain/jan_2011_calls.xlsx
@@ -3129,11 +3129,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="421200816"/>
-        <c:axId val="421198856"/>
+        <c:axId val="498577592"/>
+        <c:axId val="498577984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="421200816"/>
+        <c:axId val="498577592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3176,7 +3176,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421198856"/>
+        <c:crossAx val="498577984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3184,7 +3184,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="421198856"/>
+        <c:axId val="498577984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3235,7 +3235,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421200816"/>
+        <c:crossAx val="498577592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3545,11 +3545,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="421205912"/>
-        <c:axId val="421199640"/>
+        <c:axId val="498555640"/>
+        <c:axId val="498558776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="421205912"/>
+        <c:axId val="498555640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3592,7 +3592,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421199640"/>
+        <c:crossAx val="498558776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3600,7 +3600,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="421199640"/>
+        <c:axId val="498558776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3651,7 +3651,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421205912"/>
+        <c:crossAx val="498555640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3960,11 +3960,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="421208656"/>
-        <c:axId val="421207088"/>
+        <c:axId val="498557992"/>
+        <c:axId val="498558384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="421208656"/>
+        <c:axId val="498557992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4007,7 +4007,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421207088"/>
+        <c:crossAx val="498558384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4015,7 +4015,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="421207088"/>
+        <c:axId val="498558384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4066,7 +4066,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421208656"/>
+        <c:crossAx val="498557992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4351,11 +4351,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="421203952"/>
-        <c:axId val="421199248"/>
+        <c:axId val="498559168"/>
+        <c:axId val="498559560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="421203952"/>
+        <c:axId val="498559168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4398,7 +4398,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421199248"/>
+        <c:crossAx val="498559560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4406,7 +4406,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="421199248"/>
+        <c:axId val="498559560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4457,7 +4457,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421203952"/>
+        <c:crossAx val="498559168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7505,11 +7505,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="421201600"/>
-        <c:axId val="421203168"/>
+        <c:axId val="498557208"/>
+        <c:axId val="498549368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="421201600"/>
+        <c:axId val="498557208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7566,12 +7566,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421203168"/>
+        <c:crossAx val="498549368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="421203168"/>
+        <c:axId val="498549368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7628,7 +7628,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421201600"/>
+        <c:crossAx val="498557208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>